<commit_message>
sorting structure of test documents. wp
</commit_message>
<xml_diff>
--- a/tests/resources/cut_down_master_compared.xlsx
+++ b/tests/resources/cut_down_master_compared.xlsx
@@ -434,13 +434,15 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="B1" activeCellId="0" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A24" activeCellId="0" sqref="A24"/>
+      <selection pane="bottomRight" activeCell="F14" activeCellId="0" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="0" outlineLevelRow="0"/>
   <cols>
     <col width="59.57" customWidth="1" style="6" min="1" max="1"/>
-    <col width="8.539999999999999" customWidth="1" style="6" min="2" max="996"/>
+    <col width="8.539999999999999" customWidth="1" style="6" min="2" max="4"/>
+    <col width="10.25" customWidth="1" style="6" min="5" max="5"/>
+    <col width="8.539999999999999" customWidth="1" style="6" min="6" max="996"/>
     <col width="9.140000000000001" customWidth="1" style="6" min="997" max="1023"/>
     <col width="9.140000000000001" customWidth="1" style="6" min="1024" max="1024"/>
   </cols>
@@ -493,11 +495,11 @@
       <c r="D2" s="9" t="n">
         <v>42843</v>
       </c>
-      <c r="E2" s="10" t="n">
-        <v>42829</v>
-      </c>
-      <c r="F2" s="10" t="n">
-        <v>42832</v>
+      <c r="E2" s="9" t="n">
+        <v>42844</v>
+      </c>
+      <c r="F2" s="9" t="n">
+        <v>42845</v>
       </c>
       <c r="G2" s="10" t="n"/>
     </row>

</xml_diff>